<commit_message>
change some of the mapping as per pr feedback
</commit_message>
<xml_diff>
--- a/magda-csv-connector/src/test/csv3.xlsx
+++ b/magda-csv-connector/src/test/csv3.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Sheet1" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="owssvr" vbProcedure="false">owssvr!$A$1:$AC$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="owssvr" vbProcedure="false">owssvr!$D$1:$AF$4</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +24,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="87">
+  <si>
+    <t xml:space="preserve">Division</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Branch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Section</t>
+  </si>
   <si>
     <t xml:space="preserve">Dataset Title</t>
   </si>
@@ -111,6 +120,15 @@
   </si>
   <si>
     <t xml:space="preserve">Likelihood of release</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S</t>
   </si>
   <si>
     <t xml:space="preserve">T1</t>
@@ -382,8 +400,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_owssvr" displayName="Table_owssvr" ref="A1:AC4" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:AC4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_owssvr" displayName="Table_owssvr" ref="D1:AF4" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="D1:AF4"/>
   <tableColumns count="29">
     <tableColumn id="1" name="Dataset Title"/>
     <tableColumn id="2" name="Short Description"/>
@@ -423,51 +441,51 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AC4"/>
+  <dimension ref="A1:AF4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="78.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="39.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="47.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="8" style="0" width="78.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="14.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="78.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="46.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="78.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="12.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="16.2"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="78.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="39.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="47.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="11" style="0" width="78.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="14.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="78.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="46.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="78.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="41.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="19" style="0" width="78.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="33.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="33.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="15.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="22.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="78.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="10.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="19.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="17.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="21.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="30" style="0" width="8.23"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="12.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="16.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="78.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="41.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="22" style="0" width="78.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="33.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="33.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="15.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="22.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="78.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="10.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="19.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="17.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="21.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="33" style="0" width="8.22"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -548,211 +566,229 @@
       <c r="AC1" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>31</v>
+      <c r="A2" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>34</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="5" t="n">
         <v>41427</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="K2" s="0" t="s">
-        <v>37</v>
-      </c>
+      <c r="J2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K2" s="3"/>
       <c r="L2" s="3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="P2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="2" t="s">
+      <c r="N2" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2" t="s">
+      <c r="O2" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="P2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="V2" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="W2" s="5" t="n">
+      <c r="Q2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="T2" s="3"/>
+      <c r="U2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="X2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z2" s="5" t="n">
         <v>41640</v>
       </c>
-      <c r="X2" s="4"/>
-      <c r="Y2" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="Z2" s="4" t="s">
-        <v>47</v>
-      </c>
       <c r="AA2" s="4"/>
-      <c r="AB2" s="4" t="s">
+      <c r="AB2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD2" s="4"/>
+      <c r="AE2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="O3" s="3"/>
+      <c r="P3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="S3" s="4"/>
+      <c r="T3" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="4"/>
+      <c r="Y3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z3" s="5"/>
+      <c r="AA3" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="4"/>
+      <c r="AD3" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE3" s="4"/>
+      <c r="AF3" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="I4" s="5" t="n">
+        <v>37622</v>
+      </c>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AC2" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="I3" s="3" t="s">
+      <c r="T4" s="3"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="X4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y4" s="4"/>
+      <c r="Z4" s="5" t="n">
+        <v>42005</v>
+      </c>
+      <c r="AA4" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB4" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC4" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD4" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE4" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AF4" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="K3" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="L3" s="3"/>
-      <c r="M3" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="N3" s="3"/>
-      <c r="O3" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="4"/>
-      <c r="V3" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="W3" s="5"/>
-      <c r="X3" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="Y3" s="2"/>
-      <c r="Z3" s="4"/>
-      <c r="AA3" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB3" s="4"/>
-      <c r="AC3" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F4" s="5" t="n">
-        <v>37622</v>
-      </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="M4" s="2"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="T4" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="U4" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="V4" s="4"/>
-      <c r="W4" s="5" t="n">
-        <v>42005</v>
-      </c>
-      <c r="X4" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="Y4" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="Z4" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA4" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="AB4" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="AC4" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -783,182 +819,182 @@
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="8.22"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>